<commit_message>
Edit bug report design
</commit_message>
<xml_diff>
--- a/5- Testing/Bug Report.xlsx
+++ b/5- Testing/Bug Report.xlsx
@@ -5,15 +5,23 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dell\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dell\Documents\GitHub\Car-Purchasing-App\5- Testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C4429B2E-7085-4AF9-8CEC-F800D44E7020}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4F88942-62DE-43BC-BA5E-9400A032E6CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{56417815-FC7D-4E3F-9C7F-6BB82D9BCF1F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Add Car" sheetId="2" r:id="rId2"/>
+    <sheet name="Delete car" sheetId="3" r:id="rId3"/>
+    <sheet name="View Car" sheetId="4" r:id="rId4"/>
+    <sheet name="search" sheetId="5" r:id="rId5"/>
+    <sheet name="login" sheetId="6" r:id="rId6"/>
+    <sheet name="Logout" sheetId="7" r:id="rId7"/>
+    <sheet name="Regs" sheetId="8" r:id="rId8"/>
+    <sheet name="Reserve" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="103">
   <si>
     <t>____</t>
   </si>
@@ -71,33 +79,6 @@
   <si>
     <t>happy 
 scenario</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Manger can`t 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Add New Customer 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>the connection failed
-This is different from the requirements</t>
-    </r>
   </si>
   <si>
     <t>functional</t>
@@ -118,12 +99,705 @@
 9- Enter "Email" in Email field
 10- Press Submit button</t>
   </si>
+  <si>
+    <t>Test Data</t>
+  </si>
+  <si>
+    <t>Designed By</t>
+  </si>
+  <si>
+    <t>Assign To</t>
+  </si>
+  <si>
+    <t>Priority</t>
+  </si>
+  <si>
+    <t>severity</t>
+  </si>
+  <si>
+    <t>Expected Result</t>
+  </si>
+  <si>
+    <t>Actual Result</t>
+  </si>
+  <si>
+    <t>attachment</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Tc Related</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> Manger can`t 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve">Add New Customer 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>the connection failed
+This is different from the requirements</t>
+    </r>
+  </si>
+  <si>
+    <t>1- Customer Name = "Beshoy"
+2- Gender = "male"
+3- Date of Birth = "13-10-1998"
+4- Address = "4 st xyzbn"
+5- City = "cairo"
+6- State = "egypt"
+7- PIN = 123456
+8- Mobile Number = "01221862730"
+9- Email = "beshoysameh@gmail.com"</t>
+  </si>
+  <si>
+    <t>Beshoy</t>
+  </si>
+  <si>
+    <t>motaza</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>Major</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The system should accepts the input value 
+ and Add customer successfully
+</t>
+  </si>
+  <si>
+    <t>Add customer successfully</t>
+  </si>
+  <si>
+    <t>Screen Shot
+from Ui Desgin</t>
+  </si>
+  <si>
+    <t>20-02-2023</t>
+  </si>
+  <si>
+    <t>TC-ACFM-00</t>
+  </si>
+  <si>
+    <t>closed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Customer Name </t>
+  </si>
+  <si>
+    <t>Bug-ACFM-01</t>
+  </si>
+  <si>
+    <t>3.2-T7</t>
+  </si>
+  <si>
+    <t>When Manger Enter 
+the name in customer name field
+with space in first char the message 
+is not true
+This is different from the requirements</t>
+  </si>
+  <si>
+    <t>1- Customer Name = " Beshoy"
+2- Gender = "male"
+3- Date of Birth = "13-10-1998"
+4- Address = "4 st xyzbn"
+5- City = "cairo"
+6- State = "egypt"
+7- PIN = 123456
+8- Mobile Number = "01221862730"
+9- Email = "beshoysameh@gmail.com"</t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>Minor</t>
+  </si>
+  <si>
+    <t>system shows an error.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+First character can not have space</t>
+  </si>
+  <si>
+    <t>TC-ACFM-04</t>
+  </si>
+  <si>
+    <t>address</t>
+  </si>
+  <si>
+    <t>Bug-ACFM-02</t>
+  </si>
+  <si>
+    <t>3.2-T8</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve">Manger can Leave
+ address field </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve">blank
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>in customer data</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>This is different from the requirements</t>
+    </r>
+  </si>
+  <si>
+    <t>1- Customer Name = "Beshoy"
+2- Gender = "male"
+3- Date of Birth = "13-10-1998"
+4- Address = ""
+5- City = "cairo"
+6- State = "egypt"
+7- PIN = 123456
+8- Mobile Number = "01221862730"
+9- Email = "beshoysameh@gmail.com"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Address Field must not be blank</t>
+  </si>
+  <si>
+    <t>TC-ACFM-05</t>
+  </si>
+  <si>
+    <t>Bug-ACFM-03</t>
+  </si>
+  <si>
+    <t>3.2-T9</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve">Manger can Enter 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>address</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> value with 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve">space in first char
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> in address field
+This is different from the requirements</t>
+    </r>
+  </si>
+  <si>
+    <t>1- Customer Name = "Beshoy"
+2- Gender = "male"
+3- Date of Birth = "13-10-1998"
+4- Address = " 4 st xyzbn"
+5- City = "cairo"
+6- State = "egypt"
+7- PIN = 123456
+8- Mobile Number = "01221862730"
+9- Email = "beshoysameh@gmail.com"</t>
+  </si>
+  <si>
+    <t>hossam</t>
+  </si>
+  <si>
+    <t>TC-ACFM-06</t>
+  </si>
+  <si>
+    <t>Bug-ACFM-04</t>
+  </si>
+  <si>
+    <t>3.2-T10</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve">Manger can Enter 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>address</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> value with </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve">special char
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> in address field
+This is different from the requirements</t>
+    </r>
+  </si>
+  <si>
+    <t>1- Customer Name = "Beshoy"
+2- Gender = "male"
+3- Date of Birth = "13-10-1998"
+4- Address = " 4 @ st xyzbn"
+5- City = "cairo"
+6- State = "egypt"
+7- PIN = 123456
+8- Mobile Number = "01221862730"
+9- Email = "beshoysameh@gmail.com"</t>
+  </si>
+  <si>
+    <t>TC-ACFM-07</t>
+  </si>
+  <si>
+    <t>city</t>
+  </si>
+  <si>
+    <t>Bug-ACFM-05</t>
+  </si>
+  <si>
+    <t>3.2-T14</t>
+  </si>
+  <si>
+    <t>When Manger Enter 
+the city in city field
+with space in first char 
+the message is not true
+This is different from the requirements</t>
+  </si>
+  <si>
+    <t>1- Customer Name = " Beshoy"
+2- Gender = "male"
+3- Date of Birth = "13-10-1998"
+4- Address = "4 st xyzbn"
+5- City = " cairo"
+6- State = "egypt"
+7- PIN = 123456
+8- Mobile Number = "01221862730"
+9- Email = "beshoysameh@gmail.com"</t>
+  </si>
+  <si>
+    <t>kirollos</t>
+  </si>
+  <si>
+    <t>TC-ACFM-11</t>
+  </si>
+  <si>
+    <t>state</t>
+  </si>
+  <si>
+    <t>Bug-ACFM-06</t>
+  </si>
+  <si>
+    <t>3.2-T17.1</t>
+  </si>
+  <si>
+    <t>When Manger Enter 
+the state in state field
+with space in first char 
+the message is not true
+This is different from the requirements</t>
+  </si>
+  <si>
+    <t>1- Customer Name = " Beshoy"
+2- Gender = "male"
+3- Date of Birth = "13-10-1998"
+4- Address = "4 st xyzbn"
+5- City = "cairo"
+6- State = " egypt"
+7- PIN = 123456
+8- Mobile Number = "01221862730"
+9- Email = "beshoysameh@gmail.com"</t>
+  </si>
+  <si>
+    <t>TC-ACFM-15</t>
+  </si>
+  <si>
+    <t>PIN</t>
+  </si>
+  <si>
+    <t>Bug-ACFM-07</t>
+  </si>
+  <si>
+    <t>3.2-T22</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve">Manger can Enter 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve">pin </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve">value with 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve">space in first char
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> in pin field
+This is different from the requirements</t>
+    </r>
+  </si>
+  <si>
+    <t>1- Customer Name = " Beshoy"
+2- Gender = "male"
+3- Date of Birth = "13-10-1998"
+4- Address = "4 st xyzbn"
+5- City = "cairo"
+6- State = "egypt"
+7- PIN = " 123456"
+8- Mobile Number = "01221862730"
+9- Email = "beshoysameh@gmail.com"</t>
+  </si>
+  <si>
+    <t>nader</t>
+  </si>
+  <si>
+    <t>TC-ACFM-19</t>
+  </si>
+  <si>
+    <t>Telephone Number</t>
+  </si>
+  <si>
+    <t>Bug-ACFM-08</t>
+  </si>
+  <si>
+    <t>3.2-T26</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> Manger can Enter 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve">telephone numbe </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve">value with 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve">space in first char
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> in telephone numbe field
+This is different from the requirements</t>
+    </r>
+  </si>
+  <si>
+    <t>1- Customer Name = " Beshoy"
+2- Gender = "male"
+3- Date of Birth = "13-10-1998"
+4- Address = "4 st xyzbn"
+5- City = "cairo"
+6- State = "egypt"
+7- PIN = "123456"
+8- Mobile Number = " 01221862730"
+9- Email = "beshoysameh@gmail.com"</t>
+  </si>
+  <si>
+    <t>TC-ACFM-25</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>Bug-ACFM-09</t>
+  </si>
+  <si>
+    <t>3.2-T29</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> Manger can Enter 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve">email </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve">value with 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve">space in first char
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> in email field
+This is different from the requirements</t>
+    </r>
+  </si>
+  <si>
+    <t>1- Customer Name = "Beshoy"
+2- Gender = "male"
+3- Date of Birth = "13-10-1998"
+4- Address = "4 st xyzbn"
+5- City = "cairo"
+6- State = "egypt"
+7- PIN = "123456"
+8- Mobile Number = "01221862730"
+9- Email = " beshoysameh@gmail.com"</t>
+  </si>
+  <si>
+    <t>TC-ACFM-27</t>
+  </si>
+  <si>
+    <t>Bug-ACFM-10</t>
+  </si>
+  <si>
+    <t>3.3-F33</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve">Manger can Enter 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve">email </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>value and id is exist in sys
+This is different from the requirements</t>
+    </r>
+  </si>
+  <si>
+    <t>1- Customer Name = "Beshoy"
+2- Gender = "male"
+3- Date of Birth = "13-10-1998"
+4- Address = "4 st xyzbn"
+5- City = "cairo"
+6- State = "egypt"
+7- PIN = "123456"
+8- Mobile Number = "01221862730"
+9- Email = " moataz@gmail.com"</t>
+  </si>
+  <si>
+    <t>Email is exist please try again</t>
+  </si>
+  <si>
+    <t>TC-ACFM-28</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -136,37 +810,48 @@
       <sz val="12"/>
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="18"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="18"/>
       <color rgb="FFFF00FF"/>
       <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
-      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -176,23 +861,71 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF00FF"/>
-        <bgColor indexed="64"/>
+        <bgColor rgb="FFFF00FF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF4C1130"/>
-        <bgColor indexed="64"/>
+        <bgColor rgb="FF4C1130"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC9DAF8"/>
-        <bgColor indexed="64"/>
+        <bgColor rgb="FFC9DAF8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFE599"/>
+        <bgColor rgb="FFFFE599"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF9FC5E8"/>
+        <bgColor rgb="FF9FC5E8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF6FA8DC"/>
+        <bgColor rgb="FF6FA8DC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF3D85C6"/>
+        <bgColor rgb="FF3D85C6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0B5394"/>
+        <bgColor rgb="FF0B5394"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF073763"/>
+        <bgColor rgb="FF073763"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF351C75"/>
+        <bgColor rgb="FF351C75"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF20124D"/>
+        <bgColor rgb="FF20124D"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -201,76 +934,53 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
+      <left style="thin">
         <color rgb="FF000000"/>
       </left>
-      <right style="medium">
+      <right style="thin">
         <color rgb="FF000000"/>
       </right>
-      <top style="medium">
+      <top style="thin">
         <color rgb="FF000000"/>
       </top>
-      <bottom style="medium">
+      <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color rgb="FFCCCCCC"/>
+      <left style="thin">
+        <color rgb="FF000000"/>
       </left>
-      <right style="medium">
+      <right style="thin">
         <color rgb="FF000000"/>
       </right>
-      <top style="medium">
+      <top style="thin">
         <color rgb="FF000000"/>
       </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
+      <left style="thin">
         <color rgb="FF000000"/>
       </left>
-      <right style="medium">
+      <right style="thin">
         <color rgb="FF000000"/>
       </right>
-      <top style="medium">
-        <color rgb="FFCCCCCC"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color rgb="FFCCCCCC"/>
+      <left style="thin">
+        <color rgb="FF000000"/>
       </left>
-      <right style="medium">
-        <color rgb="FFCCCCCC"/>
-      </right>
-      <top style="medium">
-        <color rgb="FFCCCCCC"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFCCCCCC"/>
-      </left>
-      <right style="medium">
+      <right style="thin">
         <color rgb="FF000000"/>
       </right>
-      <top style="medium">
-        <color rgb="FFCCCCCC"/>
-      </top>
-      <bottom style="medium">
+      <top/>
+      <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
@@ -279,28 +989,54 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -616,10 +1352,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C53C5D38-0E20-4C50-91C1-15840653AF69}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:S12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -634,60 +1370,788 @@
     <col min="8" max="8" width="20.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="I1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="2" spans="1:8" ht="409.6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:19" ht="322.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="G2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="H2" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="7" t="s">
-        <v>14</v>
+      <c r="I2" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="O2" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="P2" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q2" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="R2" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="S2" s="8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="135.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="9"/>
+      <c r="B3" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L3" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="M3" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="N3" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="O3" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="P3" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q3" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="R3" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="S3" s="8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" ht="66" x14ac:dyDescent="0.25">
+      <c r="A4" s="9"/>
+      <c r="B4" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="K4" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L4" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="M4" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="N4" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="O4" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="P4" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q4" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="R4" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="S4" s="8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A5" s="9"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="K5" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="L5" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="M5" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="N5" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="O5" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="P5" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q5" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="R5" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="S5" s="8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A6" s="9"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="K6" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="L6" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="M6" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="N6" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="O6" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="P6" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q6" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="R6" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="S6" s="8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" ht="33" x14ac:dyDescent="0.25">
+      <c r="A7" s="9"/>
+      <c r="B7" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="K7" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="L7" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="M7" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="N7" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="O7" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="P7" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q7" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="R7" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="S7" s="8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" ht="44.25" x14ac:dyDescent="0.25">
+      <c r="A8" s="9"/>
+      <c r="B8" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="K8" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="L8" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="M8" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="N8" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="O8" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="P8" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q8" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="R8" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="S8" s="8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" ht="33" x14ac:dyDescent="0.25">
+      <c r="A9" s="9"/>
+      <c r="B9" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="K9" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="L9" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="M9" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="N9" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="O9" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="P9" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q9" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="R9" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="S9" s="8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" ht="155.25" x14ac:dyDescent="0.25">
+      <c r="A10" s="9"/>
+      <c r="B10" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="I10" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="J10" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="K10" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="L10" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="M10" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="N10" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="O10" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="P10" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q10" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="R10" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="S10" s="8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" ht="48.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="9"/>
+      <c r="B11" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="I11" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="J11" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="K11" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="L11" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="M11" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="N11" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="O11" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="P11" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q11" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="R11" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="S11" s="8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A12" s="12"/>
+      <c r="B12" s="12"/>
+      <c r="C12" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="I12" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="J12" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="K12" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="L12" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="M12" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="N12" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="O12" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="P12" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q12" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="R12" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="S12" s="8" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D66632E-9C5B-4E56-A13B-063EB1B42E22}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A18F9892-FAE7-4E20-840D-0C3A92CA19B1}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBF43E94-CAC5-4B3D-A21E-CA757A507EEF}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9822BA08-14BE-4787-AB45-722849B5D752}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2F036E8-A4B2-46D7-A52C-FD77F4B10B1E}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3336D276-0636-41D8-B830-A62A7C1E7CA6}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46AAEDC1-CF4C-4257-84A0-21471E021576}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FAE1B2E-EDFD-4D9F-B10D-208085D842D5}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>